<commit_message>
Updated foamy virus species names (removed 'fo' suffix)
</commit_message>
<xml_diff>
--- a/tabular/xrv/xrv_side_data.xlsx
+++ b/tabular/xrv/xrv_side_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/retrovirus/RVdb/tabular/xrv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1A3FEA-D3EB-D54C-9B34-0DC06B12FFE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87F3F71-DB0D-AD4E-827A-BA00E55DF995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="500" windowWidth="27200" windowHeight="16440" xr2:uid="{470E94C2-C0F7-8B49-A134-D51F9ABE93F3}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>Alpharetrovirus</t>
   </si>
   <si>
-    <t>Alpharetrovirus_avileu</t>
-  </si>
-  <si>
     <t>ALV</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>AF033808</t>
   </si>
   <si>
-    <t>Alpharetrovirus_avirousar</t>
-  </si>
-  <si>
     <t>RSV</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>Btype</t>
   </si>
   <si>
-    <t>Betaretrovirus_murmamtum</t>
-  </si>
-  <si>
     <t>MMTV</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
     <t>Dtype</t>
   </si>
   <si>
-    <t>Betaretrovirus_squmon</t>
-  </si>
-  <si>
     <t>SMRVH</t>
   </si>
   <si>
@@ -171,9 +159,6 @@
     <t>NC_001550</t>
   </si>
   <si>
-    <t>Betaretrovirus_maspfimon</t>
-  </si>
-  <si>
     <t>MPMV</t>
   </si>
   <si>
@@ -189,9 +174,6 @@
     <t>NC_001494</t>
   </si>
   <si>
-    <t>Betaretrovirus_ovijaa</t>
-  </si>
-  <si>
     <t>JSRV</t>
   </si>
   <si>
@@ -213,9 +195,6 @@
     <t>Simideltaretrovirus</t>
   </si>
   <si>
-    <t>Deltaretrovirus_priTlym1</t>
-  </si>
-  <si>
     <t>PTLV1</t>
   </si>
   <si>
@@ -231,18 +210,12 @@
     <t>NC_001488</t>
   </si>
   <si>
-    <t>Deltaretrovirus_priTlym2</t>
-  </si>
-  <si>
     <t>PTLV2</t>
   </si>
   <si>
     <t>DQ093792</t>
   </si>
   <si>
-    <t>Deltaretrovirus_priTlym3</t>
-  </si>
-  <si>
     <t>PTLV3</t>
   </si>
   <si>
@@ -252,9 +225,6 @@
     <t>EF488483</t>
   </si>
   <si>
-    <t>Deltaretrovirus_priTlym4</t>
-  </si>
-  <si>
     <t>PTLV4</t>
   </si>
   <si>
@@ -288,9 +258,6 @@
     <t>Bovilentivirus</t>
   </si>
   <si>
-    <t>Lentivirus_bovimdef</t>
-  </si>
-  <si>
     <t xml:space="preserve">BIV </t>
   </si>
   <si>
@@ -303,9 +270,6 @@
     <t>Equilentivirus</t>
   </si>
   <si>
-    <t>Lentivirus_equinfane</t>
-  </si>
-  <si>
     <t xml:space="preserve">EIAV </t>
   </si>
   <si>
@@ -324,9 +288,6 @@
     <t>Felilentivirus</t>
   </si>
   <si>
-    <t>Lentivirus_felimdef</t>
-  </si>
-  <si>
     <t>FIVP</t>
   </si>
   <si>
@@ -342,9 +303,6 @@
     <t>U21603</t>
   </si>
   <si>
-    <t>Lentivirus_bovjem</t>
-  </si>
-  <si>
     <t xml:space="preserve">JDV </t>
   </si>
   <si>
@@ -363,9 +321,6 @@
     <t>Ovilentivirus</t>
   </si>
   <si>
-    <t>Lentivirus_ovivismae</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRLVA </t>
   </si>
   <si>
@@ -378,9 +333,6 @@
     <t>M33677</t>
   </si>
   <si>
-    <t>Lentivirus_capartenc</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRLVB </t>
   </si>
   <si>
@@ -399,9 +351,6 @@
     <t>Similentivirus</t>
   </si>
   <si>
-    <t>Lentivirus_humimdef1</t>
-  </si>
-  <si>
     <t xml:space="preserve">HIV1M </t>
   </si>
   <si>
@@ -417,9 +366,6 @@
     <t>Epsilonretrovirus</t>
   </si>
   <si>
-    <t>Epsilonretrovirus_waldersar</t>
-  </si>
-  <si>
     <t>WDSV</t>
   </si>
   <si>
@@ -435,9 +381,6 @@
     <t>AF133051</t>
   </si>
   <si>
-    <t>Epsilonretrovirus_walepihyp1</t>
-  </si>
-  <si>
     <t>WEHV1</t>
   </si>
   <si>
@@ -447,9 +390,6 @@
     <t>AF133052</t>
   </si>
   <si>
-    <t>Epsilonretrovirus_walepihyp2</t>
-  </si>
-  <si>
     <t>WEHV2</t>
   </si>
   <si>
@@ -465,9 +405,6 @@
     <t>Korv_GALV</t>
   </si>
   <si>
-    <t>Gammaretrovirus_gibleu</t>
-  </si>
-  <si>
     <t>GaLV</t>
   </si>
   <si>
@@ -480,9 +417,6 @@
     <t>Gibbons</t>
   </si>
   <si>
-    <t>Gammaretrovirus_koa</t>
-  </si>
-  <si>
     <t>KoRV</t>
   </si>
   <si>
@@ -501,9 +435,6 @@
     <t>MLV_FeLV</t>
   </si>
   <si>
-    <t>Gammaretrovirus_felleu</t>
-  </si>
-  <si>
     <t>FeLV</t>
   </si>
   <si>
@@ -513,9 +444,6 @@
     <t>NC_001501</t>
   </si>
   <si>
-    <t>Gammaretrovirus_murleu</t>
-  </si>
-  <si>
     <t>MLV</t>
   </si>
   <si>
@@ -525,9 +453,6 @@
     <t>REV</t>
   </si>
   <si>
-    <t>Gammaretrovirus_aviretend</t>
-  </si>
-  <si>
     <t>Reticuloendotheliosis virus</t>
   </si>
   <si>
@@ -594,9 +519,6 @@
     <t>Bovispumavirus</t>
   </si>
   <si>
-    <t>Bovispumavirus_bostaufo</t>
-  </si>
-  <si>
     <t>BFV</t>
   </si>
   <si>
@@ -609,9 +531,6 @@
     <t>Equispumavirus</t>
   </si>
   <si>
-    <t>Equispumavirus_equcabfo</t>
-  </si>
-  <si>
     <t>EFV</t>
   </si>
   <si>
@@ -624,9 +543,6 @@
     <t>Felispumavirus</t>
   </si>
   <si>
-    <t>Felispumavirus_felcatfo</t>
-  </si>
-  <si>
     <t>FFV</t>
   </si>
   <si>
@@ -639,9 +555,6 @@
     <t>Prosimispumavirus</t>
   </si>
   <si>
-    <t>Prosimiispumavirus_otocrafo</t>
-  </si>
-  <si>
     <t>PSFVgal</t>
   </si>
   <si>
@@ -660,18 +573,12 @@
     <t>Simispumavirus</t>
   </si>
   <si>
-    <t>Simiispumavirus_maccycfo</t>
-  </si>
-  <si>
     <t>SFV1</t>
   </si>
   <si>
     <t>M74895</t>
   </si>
   <si>
-    <t>Simiispumavirus_chlaetfo</t>
-  </si>
-  <si>
     <t>SFV3</t>
   </si>
   <si>
@@ -687,9 +594,6 @@
     <t>NC_001364</t>
   </si>
   <si>
-    <t>Simiispumavirus_pantroverfo</t>
-  </si>
-  <si>
     <t>SFVcpz</t>
   </si>
   <si>
@@ -705,9 +609,6 @@
     <t>AJ544579</t>
   </si>
   <si>
-    <t>Simiispumavirus_ponpygpygfo</t>
-  </si>
-  <si>
     <t>SFVora</t>
   </si>
   <si>
@@ -723,9 +624,6 @@
     <t>Platyrhinispumavirus</t>
   </si>
   <si>
-    <t>Simiispumavirus_saiscifo</t>
-  </si>
-  <si>
     <t>SFVsqu</t>
   </si>
   <si>
@@ -735,9 +633,6 @@
     <t>NC_039027</t>
   </si>
   <si>
-    <t>Simiispumavirus_atesppfo</t>
-  </si>
-  <si>
     <t>SFVspi</t>
   </si>
   <si>
@@ -1311,9 +1206,6 @@
     <t>M74895_SFV3_RT</t>
   </si>
   <si>
-    <t>Deltaretrovirus_bovleu</t>
-  </si>
-  <si>
     <t>Alpharetrovirus avimyebla</t>
   </si>
   <si>
@@ -1332,21 +1224,6 @@
     <t>Lentivirus pum</t>
   </si>
   <si>
-    <t>Simiispumavirus sapxanfo</t>
-  </si>
-  <si>
-    <t>Simiispumavirus gorgorgorfo</t>
-  </si>
-  <si>
-    <t>Simiispumavirus macfusfo</t>
-  </si>
-  <si>
-    <t>Simiispumavirus macmulfo</t>
-  </si>
-  <si>
-    <t>Simiispumavirus macfasfo</t>
-  </si>
-  <si>
     <t>Japanese macaque</t>
   </si>
   <si>
@@ -1356,18 +1233,6 @@
     <t>Crab-eating macaque</t>
   </si>
   <si>
-    <t>Simiispumavirus pantroschfo</t>
-  </si>
-  <si>
-    <t>Simiispumavirus cernicfo</t>
-  </si>
-  <si>
-    <t>Simiispumavirus pantrotrofo</t>
-  </si>
-  <si>
-    <t>Simiispumavirus caljacfo</t>
-  </si>
-  <si>
     <t>Gammaretrovirus woomonsar</t>
   </si>
   <si>
@@ -1408,6 +1273,141 @@
   </si>
   <si>
     <t>Gammaretrovirus porConc</t>
+  </si>
+  <si>
+    <t>Simiispumavirus caljac</t>
+  </si>
+  <si>
+    <t>Simiispumavirus sapxan</t>
+  </si>
+  <si>
+    <t>Simiispumavirus gorgorgor</t>
+  </si>
+  <si>
+    <t>Simiispumavirus pantrotro</t>
+  </si>
+  <si>
+    <t>Simiispumavirus cernic</t>
+  </si>
+  <si>
+    <t>Simiispumavirus pantrosch</t>
+  </si>
+  <si>
+    <t>Simiispumavirus macfas</t>
+  </si>
+  <si>
+    <t>Simiispumavirus macmul</t>
+  </si>
+  <si>
+    <t>Simiispumavirus macfus</t>
+  </si>
+  <si>
+    <t>Deltaretrovirus bovleu</t>
+  </si>
+  <si>
+    <t>Deltaretrovirus priTlym3</t>
+  </si>
+  <si>
+    <t>Deltaretrovirus priTlym4</t>
+  </si>
+  <si>
+    <t>Deltaretrovirus priTlym2</t>
+  </si>
+  <si>
+    <t>Deltaretrovirus priTlym1</t>
+  </si>
+  <si>
+    <t>Alpharetrovirus avirousar</t>
+  </si>
+  <si>
+    <t>Alpharetrovirus avileu</t>
+  </si>
+  <si>
+    <t>Betaretrovirus murmamtum</t>
+  </si>
+  <si>
+    <t>Betaretrovirus maspfimon</t>
+  </si>
+  <si>
+    <t>Betaretrovirus squmon</t>
+  </si>
+  <si>
+    <t>Betaretrovirus ovijaa</t>
+  </si>
+  <si>
+    <t>Lentivirus bovimdef</t>
+  </si>
+  <si>
+    <t>Lentivirus bovjem</t>
+  </si>
+  <si>
+    <t>Lentivirus equinfane</t>
+  </si>
+  <si>
+    <t>Lentivirus felimdef</t>
+  </si>
+  <si>
+    <t>Lentivirus capartenc</t>
+  </si>
+  <si>
+    <t>Lentivirus ovivismae</t>
+  </si>
+  <si>
+    <t>Lentivirus humimdef1</t>
+  </si>
+  <si>
+    <t>Epsilonretrovirus waldersar</t>
+  </si>
+  <si>
+    <t>Epsilonretrovirus walepihyp1</t>
+  </si>
+  <si>
+    <t>Epsilonretrovirus walepihyp2</t>
+  </si>
+  <si>
+    <t>Gammaretrovirus koa</t>
+  </si>
+  <si>
+    <t>Gammaretrovirus gibleu</t>
+  </si>
+  <si>
+    <t>Gammaretrovirus murleu</t>
+  </si>
+  <si>
+    <t>Gammaretrovirus felleu</t>
+  </si>
+  <si>
+    <t>Gammaretrovirus aviretend</t>
+  </si>
+  <si>
+    <t>Bovispumavirus bostau</t>
+  </si>
+  <si>
+    <t>Equispumavirus equcab</t>
+  </si>
+  <si>
+    <t>Felispumavirus felcat</t>
+  </si>
+  <si>
+    <t>Simiispumavirus atespp</t>
+  </si>
+  <si>
+    <t>Simiispumavirus saisci</t>
+  </si>
+  <si>
+    <t>Prosimiispumavirus otocra</t>
+  </si>
+  <si>
+    <t>Simiispumavirus ponpygpyg</t>
+  </si>
+  <si>
+    <t>Simiispumavirus chlaet</t>
+  </si>
+  <si>
+    <t>Simiispumavirus pantrover</t>
+  </si>
+  <si>
+    <t>Simiispumavirus maccyc</t>
   </si>
 </sst>
 </file>
@@ -1880,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258DBE79-6346-994D-A21D-DCB1F38B2A46}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="N5" sqref="A1:N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1903,13 +1903,13 @@
   <sheetData>
     <row r="1" spans="1:16" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>379</v>
+        <v>344</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>380</v>
+        <v>345</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>6</v>
@@ -1918,19 +1918,19 @@
         <v>5</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>410</v>
+        <v>375</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>413</v>
+        <v>378</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>1</v>
@@ -1947,25 +1947,25 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>341</v>
+        <v>306</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H2" s="3">
         <v>8419</v>
@@ -1974,42 +1974,42 @@
         <v>10</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>342</v>
+        <v>307</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H3" s="3">
         <v>8917</v>
@@ -2018,40 +2018,40 @@
         <v>10</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>68</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>343</v>
+        <v>308</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H4" s="3">
         <v>8791</v>
@@ -2060,42 +2060,42 @@
         <v>10</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>72</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>344</v>
+        <v>309</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H5" s="3">
         <v>8952</v>
@@ -2104,42 +2104,42 @@
         <v>10</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>65</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>345</v>
+        <v>310</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H6" s="3">
         <v>9028</v>
@@ -2148,42 +2148,42 @@
         <v>10</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>59</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="H7" s="3">
         <v>9392</v>
@@ -2192,7 +2192,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>12</v>
@@ -2202,30 +2202,30 @@
       </c>
       <c r="M7" s="9"/>
       <c r="N7" s="9" t="s">
-        <v>19</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>347</v>
+        <v>312</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="H8" s="3">
         <v>7286</v>
@@ -2234,7 +2234,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>12</v>
@@ -2244,28 +2244,28 @@
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="9" t="s">
-        <v>14</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>348</v>
+        <v>313</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="H9" s="3">
         <v>7143</v>
@@ -2274,7 +2274,7 @@
         <v>10</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>12</v>
@@ -2284,30 +2284,30 @@
       </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="H10" s="3">
         <v>8805</v>
@@ -2316,42 +2316,42 @@
         <v>10</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>30</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H11" s="3">
         <v>8557</v>
@@ -2360,40 +2360,40 @@
         <v>10</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>45</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H12" s="3">
         <v>8173</v>
@@ -2402,42 +2402,42 @@
         <v>10</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>352</v>
+        <v>317</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H13" s="3">
         <v>8785</v>
@@ -2446,42 +2446,42 @@
         <v>10</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>37</v>
+        <v>431</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H14" s="3">
         <v>7462</v>
@@ -2490,42 +2490,42 @@
         <v>10</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>51</v>
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>420</v>
+        <v>385</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>323</v>
+        <v>288</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H15" s="3">
         <v>8482</v>
@@ -2534,42 +2534,42 @@
         <v>10</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>84</v>
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>419</v>
+        <v>384</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>326</v>
+        <v>291</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="H16" s="3">
         <v>7732</v>
@@ -2578,40 +2578,40 @@
         <v>10</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>102</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>418</v>
+        <v>383</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="H17" s="3">
         <v>8407</v>
@@ -2620,40 +2620,40 @@
         <v>10</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>89</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>421</v>
+        <v>386</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="H18" s="3">
         <v>9474</v>
@@ -2662,42 +2662,42 @@
         <v>10</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>96</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>324</v>
+        <v>289</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>335</v>
+        <v>300</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>402</v>
+        <v>367</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>401</v>
+        <v>366</v>
       </c>
       <c r="H19" s="3">
         <v>9100</v>
@@ -2706,40 +2706,40 @@
         <v>10</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>431</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>422</v>
+        <v>387</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="H20" s="3">
         <v>9189</v>
@@ -2748,40 +2748,40 @@
         <v>10</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>114</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>423</v>
+        <v>388</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="H21" s="3">
         <v>9221</v>
@@ -2790,80 +2790,80 @@
         <v>10</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>109</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>417</v>
+        <v>382</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="9" t="s">
         <v>10</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>121</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>355</v>
+        <v>320</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>336</v>
+        <v>301</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H23" s="3">
         <v>10359</v>
@@ -2872,38 +2872,38 @@
         <v>10</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>429</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>356</v>
+        <v>321</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="3" t="s">
-        <v>400</v>
+        <v>365</v>
       </c>
       <c r="H24" s="3">
         <v>9623</v>
@@ -2912,42 +2912,42 @@
         <v>10</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>430</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="H25" s="3">
         <v>12708</v>
@@ -2956,38 +2956,38 @@
         <v>10</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9" t="s">
-        <v>127</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>358</v>
+        <v>323</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="H26" s="3">
         <v>12999</v>
@@ -2996,38 +2996,38 @@
         <v>10</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="M26" s="9"/>
       <c r="N26" s="9" t="s">
-        <v>133</v>
+        <v>441</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>359</v>
+        <v>324</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="H27" s="3">
         <v>13125</v>
@@ -3036,40 +3036,40 @@
         <v>10</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="9" t="s">
-        <v>137</v>
+        <v>442</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>360</v>
+        <v>325</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="H28" s="3">
         <v>8431</v>
@@ -3078,42 +3078,42 @@
         <v>10</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>148</v>
+        <v>443</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>361</v>
+        <v>326</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="H29" s="3">
         <v>8088</v>
@@ -3122,42 +3122,42 @@
         <v>10</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>143</v>
+        <v>444</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>362</v>
+        <v>327</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H30" s="3">
         <v>8332</v>
@@ -3166,42 +3166,42 @@
         <v>10</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>159</v>
+        <v>445</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>363</v>
+        <v>328</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="H31" s="3">
         <v>8448</v>
@@ -3210,42 +3210,42 @@
         <v>10</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>155</v>
+        <v>446</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>364</v>
+        <v>329</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="H32" s="3">
         <v>8295</v>
@@ -3254,40 +3254,40 @@
         <v>10</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>163</v>
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>365</v>
+        <v>330</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="H33" s="3">
         <v>8389</v>
@@ -3296,40 +3296,40 @@
         <v>10</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M33" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="M33" s="9" t="s">
-        <v>166</v>
-      </c>
       <c r="N33" s="9" t="s">
-        <v>163</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>381</v>
+        <v>346</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>398</v>
+        <v>363</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>397</v>
+        <v>362</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>399</v>
+        <v>364</v>
       </c>
       <c r="H34" s="3">
         <v>8072</v>
@@ -3338,40 +3338,40 @@
         <v>10</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="M34" s="9"/>
       <c r="N34" s="9" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>366</v>
+        <v>331</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="H35" s="3">
         <v>10305</v>
@@ -3380,38 +3380,38 @@
         <v>10</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="M35" s="9"/>
       <c r="N35" s="9" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>367</v>
+        <v>332</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="H36" s="3">
         <v>10688</v>
@@ -3420,40 +3420,40 @@
         <v>10</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="M36" s="9"/>
       <c r="N36" s="9" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>368</v>
+        <v>333</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>325</v>
+        <v>290</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H37" s="3">
         <v>12002</v>
@@ -3462,42 +3462,42 @@
         <v>10</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>186</v>
+        <v>448</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="H38" s="3">
         <v>12035</v>
@@ -3506,42 +3506,42 @@
         <v>10</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>191</v>
+        <v>449</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>370</v>
+        <v>335</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>327</v>
+        <v>292</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="H39" s="3">
         <v>11700</v>
@@ -3550,42 +3550,42 @@
         <v>10</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>196</v>
+        <v>450</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>371</v>
+        <v>336</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="H40" s="3">
         <v>12212</v>
@@ -3594,42 +3594,42 @@
         <v>10</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>233</v>
+        <v>451</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>372</v>
+        <v>337</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H41" s="3">
         <v>11684</v>
@@ -3638,42 +3638,42 @@
         <v>10</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M41" s="9" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>229</v>
+        <v>452</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>377</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>412</v>
       </c>
       <c r="H42" s="3">
         <v>11744</v>
@@ -3682,40 +3682,40 @@
         <v>10</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>443</v>
+        <v>413</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>385</v>
+        <v>350</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>395</v>
+        <v>360</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>403</v>
+        <v>368</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>404</v>
+        <v>369</v>
       </c>
       <c r="H43" s="3">
         <v>11764</v>
@@ -3724,42 +3724,42 @@
         <v>10</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M43" s="9" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>373</v>
+        <v>338</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="H44" s="3">
         <v>12118</v>
@@ -3768,42 +3768,42 @@
         <v>10</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="N44" s="9" t="s">
-        <v>201</v>
+        <v>453</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>374</v>
+        <v>339</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>224</v>
+        <v>191</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="H45" s="3">
         <v>12823</v>
@@ -3812,40 +3812,40 @@
         <v>10</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>223</v>
+        <v>454</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>424</v>
+        <v>389</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="H46" s="3">
         <v>13111</v>
@@ -3854,42 +3854,42 @@
         <v>10</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N46" s="9" t="s">
-        <v>211</v>
+        <v>455</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>375</v>
+        <v>340</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="H47" s="3">
         <v>13246</v>
@@ -3898,40 +3898,40 @@
         <v>10</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L47" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M47" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N47" s="9" t="s">
-        <v>217</v>
+        <v>456</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H48" s="3">
         <v>12972</v>
@@ -3940,42 +3940,42 @@
         <v>10</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L48" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N48" s="9" t="s">
-        <v>208</v>
+        <v>457</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>378</v>
+        <v>343</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>339</v>
+        <v>304</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>396</v>
+        <v>361</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>409</v>
+        <v>374</v>
       </c>
       <c r="H49" s="3">
         <v>12258</v>
@@ -3984,40 +3984,40 @@
         <v>10</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M49" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N49" s="9" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>386</v>
+        <v>351</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>329</v>
+        <v>294</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>389</v>
+        <v>354</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>408</v>
+        <v>373</v>
       </c>
       <c r="H50" s="3">
         <v>13220</v>
@@ -4026,42 +4026,42 @@
         <v>10</v>
       </c>
       <c r="J50" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L50" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="M50" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="N50" s="9" t="s">
         <v>416</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="L50" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="N50" s="9" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>384</v>
+        <v>349</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>328</v>
+        <v>293</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>390</v>
+        <v>355</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>406</v>
+        <v>371</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>407</v>
+        <v>372</v>
       </c>
       <c r="H51" s="3">
         <v>13072</v>
@@ -4070,40 +4070,40 @@
         <v>10</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M51" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N51" s="9" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>387</v>
+        <v>352</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>391</v>
+        <v>356</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="H52" s="3">
         <v>11954</v>
@@ -4112,40 +4112,40 @@
         <v>10</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L52" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M52" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N52" s="9" t="s">
-        <v>440</v>
+        <v>418</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>388</v>
+        <v>353</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>392</v>
+        <v>357</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>438</v>
+        <v>397</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>439</v>
+        <v>398</v>
       </c>
       <c r="H53" s="3">
         <v>12965</v>
@@ -4154,40 +4154,40 @@
         <v>10</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M53" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N53" s="9" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>383</v>
+        <v>348</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>393</v>
+        <v>358</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H54" s="3">
         <v>12983</v>
@@ -4196,40 +4196,40 @@
         <v>10</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L54" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M54" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N54" s="9" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>382</v>
+        <v>347</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>394</v>
+        <v>359</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>405</v>
+        <v>370</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>437</v>
+        <v>396</v>
       </c>
       <c r="H55" s="3">
         <v>12957</v>
@@ -4238,19 +4238,19 @@
         <v>10</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>416</v>
+        <v>381</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="M55" s="9" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="N55" s="9" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.2">
@@ -4318,25 +4318,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>379</v>
+        <v>344</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>380</v>
+        <v>345</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>413</v>
+        <v>378</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -4362,12 +4362,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="E2" s="5">
         <v>3392</v>
@@ -4382,7 +4382,7 @@
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>428</v>
+        <v>392</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -4392,12 +4392,12 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="E3" s="5">
         <v>4788</v>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>427</v>
+        <v>391</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -4422,12 +4422,12 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="E4" s="5">
         <v>1248</v>
@@ -4438,11 +4438,11 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>446</v>
+        <v>401</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -4452,12 +4452,12 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
       <c r="E5" s="5">
         <v>1928</v>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
-        <v>426</v>
+        <v>390</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -4482,12 +4482,12 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="E6" s="5">
         <v>997</v>
@@ -4498,11 +4498,11 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>447</v>
+        <v>402</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -4512,12 +4512,12 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="E7" s="5">
         <v>3811</v>
@@ -4528,11 +4528,11 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>445</v>
+        <v>400</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -4542,12 +4542,12 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="E8" s="5">
         <v>5188</v>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="14" t="s">
-        <v>456</v>
+        <v>411</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -4572,12 +4572,12 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="E9" s="5">
         <v>3166</v>
@@ -4592,7 +4592,7 @@
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>448</v>
+        <v>403</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -4602,12 +4602,12 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="E10" s="5">
         <v>2630</v>
@@ -4622,7 +4622,7 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>449</v>
+        <v>404</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -4632,12 +4632,12 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="E11" s="5">
         <v>4901</v>
@@ -4648,11 +4648,11 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>451</v>
+        <v>406</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -4662,12 +4662,12 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>315</v>
+        <v>280</v>
       </c>
       <c r="E12" s="5">
         <v>1329</v>
@@ -4678,11 +4678,11 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>450</v>
+        <v>405</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -4692,12 +4692,12 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>316</v>
+        <v>281</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="E13" s="5">
         <v>2473</v>
@@ -4708,11 +4708,11 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>455</v>
+        <v>410</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -4722,12 +4722,12 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>319</v>
+        <v>284</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="E14" s="5">
         <v>2428</v>
@@ -4742,7 +4742,7 @@
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>454</v>
+        <v>409</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -4752,12 +4752,12 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="E15" s="5">
         <v>5833</v>
@@ -4768,11 +4768,11 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>452</v>
+        <v>407</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -4782,12 +4782,12 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="E16" s="5">
         <v>266</v>
@@ -4802,13 +4802,13 @@
         <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>453</v>
+        <v>408</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -4816,12 +4816,12 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="E17" s="5">
         <v>5779</v>
@@ -4830,17 +4830,17 @@
         <v>10</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>444</v>
+        <v>399</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>

</xml_diff>

<commit_message>
Update phylogeny with reduced taxa set
</commit_message>
<xml_diff>
--- a/tabular/xrv/xrv_side_data.xlsx
+++ b/tabular/xrv/xrv_side_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/retrovirus/RVdb/tabular/xrv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC632697-26DA-CB4B-8217-46E9627BE71A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C84E17F-6769-E64F-B8B1-FCA9566BBBFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="500" windowWidth="20000" windowHeight="17500" xr2:uid="{470E94C2-C0F7-8B49-A134-D51F9ABE93F3}"/>
+    <workbookView xWindow="2460" yWindow="500" windowWidth="24420" windowHeight="15440" xr2:uid="{470E94C2-C0F7-8B49-A134-D51F9ABE93F3}"/>
   </bookViews>
   <sheets>
     <sheet name="RT species" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="295">
   <si>
     <t>subfamily</t>
   </si>
@@ -122,12 +122,6 @@
     <t>PTLV3</t>
   </si>
   <si>
-    <t>EF488483</t>
-  </si>
-  <si>
-    <t>PTLV4</t>
-  </si>
-  <si>
     <t>NC_001414</t>
   </si>
   <si>
@@ -476,9 +470,6 @@
     <t>DQ093792_PTLV3_RT</t>
   </si>
   <si>
-    <t>EF488483_PTLV4_RT</t>
-  </si>
-  <si>
     <t>M10060_PTLV2_RT</t>
   </si>
   <si>
@@ -704,9 +695,6 @@
     <t>Deltaretrovirus priTlym3</t>
   </si>
   <si>
-    <t>Deltaretrovirus priTlym4</t>
-  </si>
-  <si>
     <t>Deltaretrovirus priTlym2</t>
   </si>
   <si>
@@ -891,9 +879,6 @@
   </si>
   <si>
     <t>primate T-lymphotropic virus 3</t>
-  </si>
-  <si>
-    <t>primate T-lymphotropic virus 4</t>
   </si>
   <si>
     <t>human T-lymphotropic virus 2</t>
@@ -939,7 +924,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -953,14 +938,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -993,7 +970,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1018,12 +995,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1037,20 +1008,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1365,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258DBE79-6346-994D-A21D-DCB1F38B2A46}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:K50"/>
+    <sheetView tabSelected="1" topLeftCell="G34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K49" sqref="A1:K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1377,77 +1347,77 @@
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="40.1640625" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17" style="8" customWidth="1"/>
-    <col min="10" max="10" width="24.1640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="17" style="7" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>110</v>
+      <c r="K1" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>221</v>
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>218</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="2">
         <v>8419</v>
       </c>
@@ -1457,193 +1427,195 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>222</v>
+      <c r="F3" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="2">
         <v>8917</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>223</v>
+        <v>282</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>220</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="2">
-        <v>8791</v>
+        <v>8952</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>224</v>
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>221</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="4"/>
       <c r="K5" s="2">
-        <v>8952</v>
+        <v>9028</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>288</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>225</v>
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="2">
-        <v>9028</v>
+        <v>9392</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>284</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>226</v>
+        <v>8</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="2">
-        <v>9392</v>
+        <v>7286</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>227</v>
+        <v>14</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="4"/>
       <c r="K8" s="2">
-        <v>7286</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1651,65 +1623,65 @@
         <v>94</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>290</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>228</v>
+        <v>18</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="2">
-        <v>8805</v>
+        <v>8557</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>286</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>229</v>
+        <v>16</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="4"/>
       <c r="K10" s="2">
-        <v>8557</v>
+        <v>8785</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1717,131 +1689,129 @@
         <v>95</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>291</v>
+        <v>122</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>230</v>
+        <v>21</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="4"/>
       <c r="K11" s="2">
-        <v>8785</v>
+        <v>7462</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>231</v>
+        <v>33</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="4"/>
       <c r="K12" s="2">
-        <v>7462</v>
+        <v>8482</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>283</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>232</v>
+        <v>39</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="4"/>
       <c r="K13" s="2">
-        <v>8482</v>
+        <v>7732</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>131</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>233</v>
+        <v>35</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="4"/>
       <c r="K14" s="2">
-        <v>7732</v>
+        <v>8407</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1853,276 +1823,276 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>234</v>
+      <c r="F15" s="4" t="s">
+        <v>231</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="4"/>
       <c r="K15" s="2">
-        <v>8407</v>
+        <v>9474</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>235</v>
+        <v>137</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="4"/>
       <c r="K16" s="2">
-        <v>9474</v>
+        <v>9100</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>126</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>210</v>
+        <v>44</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>232</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="4"/>
       <c r="K17" s="2">
-        <v>9100</v>
+        <v>9189</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>236</v>
+        <v>42</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="4"/>
       <c r="K18" s="2">
-        <v>9189</v>
+        <v>9221</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>237</v>
+        <v>46</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="2">
-        <v>9221</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>200</v>
+        <v>154</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="2"/>
+      <c r="I20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="2">
+        <v>10359</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>208</v>
+        <v>139</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="4"/>
       <c r="K21" s="2">
-        <v>10359</v>
+        <v>9623</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>209</v>
+        <v>50</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="4"/>
       <c r="K22" s="2">
-        <v>9623</v>
+        <v>12708</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>239</v>
+      <c r="F23" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" s="4"/>
       <c r="K23" s="2">
-        <v>12708</v>
+        <v>12999</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -2130,160 +2100,162 @@
         <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>240</v>
+      <c r="F24" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J24" s="4"/>
       <c r="K24" s="2">
-        <v>12999</v>
+        <v>13125</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C25" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="D25" s="2" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="5"/>
+      <c r="J25" s="4"/>
       <c r="K25" s="2">
-        <v>13125</v>
+        <v>8431</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>242</v>
+        <v>57</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J26" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="4"/>
       <c r="K26" s="2">
-        <v>8431</v>
+        <v>8088</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>279</v>
+        <v>110</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>243</v>
+        <v>62</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>240</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J27" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="4"/>
       <c r="K27" s="2">
-        <v>8088</v>
+        <v>8332</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>244</v>
+        <v>60</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J28" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="4"/>
       <c r="K28" s="2">
-        <v>8332</v>
+        <v>8448</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -2291,774 +2263,741 @@
         <v>104</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>245</v>
+        <v>64</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J29" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29" s="4"/>
       <c r="K29" s="2">
-        <v>8448</v>
+        <v>8295</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>246</v>
+        <v>192</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J30" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="4"/>
       <c r="K30" s="2">
-        <v>8295</v>
+        <v>8072</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>276</v>
+        <v>164</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>211</v>
+        <v>69</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>243</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="J31" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="K31" s="2">
-        <v>8072</v>
+        <v>12002</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>258</v>
+        <v>132</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>253</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="K32" s="2">
-        <v>12002</v>
+        <v>12035</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>257</v>
+        <v>130</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>255</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="K33" s="2">
-        <v>12035</v>
+        <v>11700</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>259</v>
+        <v>89</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>256</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>249</v>
+        <v>90</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>76</v>
+      <c r="J34" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K34" s="2">
-        <v>11700</v>
+        <v>12212</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>260</v>
+        <v>134</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>267</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>250</v>
+        <v>88</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>81</v>
+      <c r="J35" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K35" s="2">
-        <v>12212</v>
+        <v>11684</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>271</v>
+      <c r="D36" s="8" t="s">
+        <v>258</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>251</v>
+        <v>140</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>81</v>
+      <c r="J36" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K36" s="2">
-        <v>11684</v>
+        <v>11744</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>262</v>
+        <v>181</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="8" t="s">
+        <v>268</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>212</v>
+        <v>191</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>81</v>
+      <c r="J37" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K37" s="2">
-        <v>11744</v>
+        <v>11764</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="9" t="s">
-        <v>272</v>
+        <v>169</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>213</v>
+        <v>77</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>81</v>
+      <c r="J38" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K38" s="2">
-        <v>11764</v>
+        <v>12118</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>261</v>
+        <v>135</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>269</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="K39" s="2">
-        <v>12118</v>
+        <v>12823</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>273</v>
+        <v>204</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="8" t="s">
+        <v>260</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>253</v>
+        <v>82</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I40" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>81</v>
+      <c r="J40" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K40" s="2">
-        <v>12823</v>
+        <v>13111</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="9" t="s">
-        <v>264</v>
+      <c r="D41" s="8" t="s">
+        <v>270</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>254</v>
+      <c r="F41" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>81</v>
+      <c r="J41" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K41" s="2">
-        <v>13111</v>
+        <v>13246</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>274</v>
+        <v>172</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="8" t="s">
+        <v>262</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>255</v>
+        <v>80</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>252</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>81</v>
+      <c r="J42" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K42" s="2">
-        <v>13246</v>
+        <v>12972</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="9" t="s">
-        <v>266</v>
+        <v>174</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>261</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>256</v>
+        <v>141</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>211</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>81</v>
+      <c r="J43" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K43" s="2">
-        <v>12972</v>
+        <v>12258</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K44" s="2">
+        <v>13220</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H44" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I45" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I44" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K44" s="2">
-        <v>12258</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>81</v>
+      <c r="J45" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K45" s="2">
-        <v>13220</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.25">
+        <v>13072</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>263</v>
+      <c r="C46" s="2"/>
+      <c r="D46" s="8" t="s">
+        <v>266</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>216</v>
+        <v>187</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I46" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>81</v>
+      <c r="J46" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K46" s="2">
-        <v>13072</v>
+        <v>11954</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="9" t="s">
-        <v>270</v>
+      <c r="D47" s="8" t="s">
+        <v>263</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>217</v>
+        <v>188</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>81</v>
+      <c r="J47" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K47" s="2">
-        <v>11954</v>
+        <v>12965</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="9" t="s">
-        <v>267</v>
+      <c r="D48" s="8" t="s">
+        <v>264</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>218</v>
+        <v>189</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>216</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I48" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>81</v>
+      <c r="J48" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K48" s="2">
-        <v>12965</v>
+        <v>12983</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="9" t="s">
-        <v>268</v>
+      <c r="D49" s="8" t="s">
+        <v>265</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>219</v>
+        <v>190</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H49" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I49" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I49" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>81</v>
+      <c r="J49" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="K49" s="2">
-        <v>12983</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K50" s="2">
         <v>12957</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J50">
-    <sortCondition ref="H2:H50"/>
-    <sortCondition ref="I2:I50"/>
-    <sortCondition ref="J2:J50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J49">
+    <sortCondition ref="H2:H49"/>
+    <sortCondition ref="I2:I49"/>
+    <sortCondition ref="J2:J49"/>
   </sortState>
   <dataValidations count="7">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B7 B4:B5 E7 E4:E5" xr:uid="{5A08E3ED-D91F-6C43-9B8E-FC55A255ED89}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B6 E6 E4 B4" xr:uid="{5A08E3ED-D91F-6C43-9B8E-FC55A255ED89}">
       <formula1>OR(LEFT(#REF!,LEN(#REF!))=#REF!,#REF!="Species")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="E7" xr:uid="{6E1AF704-BB33-8940-B9DD-861103386334}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="E6" xr:uid="{6E1AF704-BB33-8940-B9DD-861103386334}">
       <formula1>OR(LEFT(E1,LEN(L1))=L1,E1="Species")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="E8" xr:uid="{FAF04538-F137-2448-AEBE-90AC95C1E508}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="E7" xr:uid="{FAF04538-F137-2448-AEBE-90AC95C1E508}">
       <formula1>OR(LEFT(E3,LEN(L2))=L2,E3="Species")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="E6" xr:uid="{F3E3D4F1-5432-D94C-BAF1-1EB768E3EDB1}">
-      <formula1>OR(LEFT(E4,LEN(L3))=L3,E4="Species")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="E5" xr:uid="{F3E3D4F1-5432-D94C-BAF1-1EB768E3EDB1}">
+      <formula1>OR(LEFT(#REF!,LEN(L3))=L3,#REF!="Species")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B7" xr:uid="{71D6C4F5-ACFA-4844-B818-5EE2E95DDB73}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B6" xr:uid="{71D6C4F5-ACFA-4844-B818-5EE2E95DDB73}">
       <formula1>OR(LEFT(B1,LEN(J1))=J1,B1="Species")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B8" xr:uid="{7AD80CE6-3528-9441-A812-DE4763086A99}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B7" xr:uid="{7AD80CE6-3528-9441-A812-DE4763086A99}">
       <formula1>OR(LEFT(B3,LEN(J2))=J2,B3="Species")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B6" xr:uid="{7CA93BF4-0F53-BE49-8D6A-042F0360F61F}">
-      <formula1>OR(LEFT(B4,LEN(J3))=J3,B4="Species")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Binomial Naming" error="Species name must start with the name of it's genus." promptTitle="binomial" sqref="B5" xr:uid="{7CA93BF4-0F53-BE49-8D6A-042F0360F61F}">
+      <formula1>OR(LEFT(#REF!,LEN(J3))=J3,#REF!="Species")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correct subgenus for prosimian foamy virus
</commit_message>
<xml_diff>
--- a/tabular/xrv/xrv_side_data.xlsx
+++ b/tabular/xrv/xrv_side_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/retrovirus/RVdb/tabular/xrv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1C82E8-C7CC-5149-A673-775F69BE8F89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC9D36D-523A-E44B-891D-9FD33AF859E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="500" windowWidth="24420" windowHeight="15440" xr2:uid="{470E94C2-C0F7-8B49-A134-D51F9ABE93F3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="296">
   <si>
     <t>subfamily</t>
   </si>
@@ -918,6 +918,9 @@
   </si>
   <si>
     <t>puma lentivirus 14</t>
+  </si>
+  <si>
+    <t>Prosimiispumavirus</t>
   </si>
 </sst>
 </file>
@@ -1337,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258DBE79-6346-994D-A21D-DCB1F38B2A46}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:K49"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,22 +1394,22 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>280</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>194</v>
@@ -1415,29 +1418,31 @@
         <v>48</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2">
-        <v>8419</v>
+        <v>9392</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>194</v>
@@ -1446,31 +1451,31 @@
         <v>48</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="2">
-        <v>8917</v>
+        <v>7286</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>194</v>
@@ -1479,31 +1484,31 @@
         <v>48</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="2">
-        <v>8952</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>283</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>194</v>
@@ -1512,31 +1517,31 @@
         <v>48</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="2">
-        <v>9028</v>
+        <v>8557</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>286</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>194</v>
@@ -1545,31 +1550,31 @@
         <v>48</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="2">
-        <v>9392</v>
+        <v>8785</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>284</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>194</v>
@@ -1578,31 +1583,31 @@
         <v>48</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="2">
-        <v>7286</v>
+        <v>7462</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>194</v>
@@ -1611,31 +1616,29 @@
         <v>48</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="2">
-        <v>8805</v>
+        <v>8419</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>281</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>194</v>
@@ -1644,31 +1647,31 @@
         <v>48</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="2">
-        <v>8557</v>
+        <v>8917</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>194</v>
@@ -1677,31 +1680,31 @@
         <v>48</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="2">
-        <v>8785</v>
+        <v>8952</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>122</v>
+        <v>283</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>194</v>
@@ -1710,312 +1713,322 @@
         <v>48</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="2">
-        <v>7462</v>
+        <v>9028</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="2">
-        <v>8482</v>
+        <v>12708</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>277</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="2">
-        <v>7732</v>
+        <v>12999</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="2">
-        <v>8407</v>
+        <v>13125</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="2">
-        <v>9474</v>
+        <v>8431</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>137</v>
+        <v>57</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="2">
-        <v>9100</v>
+        <v>8088</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>289</v>
+        <v>110</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="2">
-        <v>9189</v>
+        <v>8332</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>162</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="2">
-        <v>9221</v>
+        <v>8448</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J19" s="4"/>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2">
+        <v>8295</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>138</v>
+        <v>192</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="2">
-        <v>10359</v>
+        <v>8072</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>200</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>194</v>
@@ -2028,298 +2041,288 @@
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="2">
-        <v>9623</v>
+        <v>8482</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>292</v>
+        <v>40</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="2">
-        <v>12708</v>
+        <v>7732</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="2">
-        <v>12999</v>
+        <v>8407</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="2">
-        <v>13125</v>
+        <v>9474</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>58</v>
+        <v>137</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="2">
-        <v>8431</v>
+        <v>9100</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="2">
-        <v>8088</v>
+        <v>9189</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>110</v>
+        <v>290</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="2">
-        <v>8332</v>
+        <v>9221</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="J28" s="4"/>
-      <c r="K28" s="2">
-        <v>8448</v>
-      </c>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>63</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="2">
-        <v>8295</v>
+        <v>10359</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>272</v>
+        <v>293</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>192</v>
+        <v>139</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>48</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="2">
-        <v>8072</v>
+        <v>9623</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -2429,22 +2432,22 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>196</v>
@@ -2456,30 +2459,30 @@
         <v>67</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>79</v>
+        <v>295</v>
       </c>
       <c r="K34" s="2">
-        <v>12212</v>
+        <v>12118</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>196</v>
@@ -2494,27 +2497,27 @@
         <v>79</v>
       </c>
       <c r="K35" s="2">
-        <v>11684</v>
+        <v>12212</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>196</v>
@@ -2529,25 +2532,27 @@
         <v>79</v>
       </c>
       <c r="K36" s="2">
-        <v>11744</v>
+        <v>11684</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C37" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="D37" s="8" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>191</v>
+        <v>140</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>196</v>
@@ -2562,27 +2567,25 @@
         <v>79</v>
       </c>
       <c r="K37" s="2">
-        <v>11764</v>
+        <v>11744</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>76</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="8" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>196</v>
@@ -2597,7 +2600,7 @@
         <v>79</v>
       </c>
       <c r="K38" s="2">
-        <v>12118</v>
+        <v>11764</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2972,7 +2975,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J49">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K49">
     <sortCondition ref="H2:H49"/>
     <sortCondition ref="I2:I49"/>
     <sortCondition ref="J2:J49"/>

</xml_diff>